<commit_message>
How to configurate the Google sheets API to storage user's information
</commit_message>
<xml_diff>
--- a/files/template.xlsx
+++ b/files/template.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrocapriles/Documents/courses/platzi/javascript/whatsapp-integration/medpet-chatbot-service/files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A04B48-4B83-C143-B481-954C5BE1F53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja 1" sheetId="1" r:id="rId4"/>
+    <sheet name="books" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -34,16 +43,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -54,111 +64,103 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEEF7E3"/>
+          <bgColor rgb="FFEEF7E3"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF8BC34A"/>
           <bgColor rgb="FF8BC34A"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEEF7E3"/>
-          <bgColor rgb="FFEEF7E3"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Hoja 1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Hoja 1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" headerRowCount="0" ref="A1:Z1" displayName="Table_1" name="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:Z1" headerRowCount="0">
   <tableColumns count="26">
-    <tableColumn name="Column1" id="1"/>
-    <tableColumn name="Column2" id="2"/>
-    <tableColumn name="Column3" id="3"/>
-    <tableColumn name="Column4" id="4"/>
-    <tableColumn name="Column5" id="5"/>
-    <tableColumn name="Column6" id="6"/>
-    <tableColumn name="Column7" id="7"/>
-    <tableColumn name="Column8" id="8"/>
-    <tableColumn name="Column9" id="9"/>
-    <tableColumn name="Column10" id="10"/>
-    <tableColumn name="Column11" id="11"/>
-    <tableColumn name="Column12" id="12"/>
-    <tableColumn name="Column13" id="13"/>
-    <tableColumn name="Column14" id="14"/>
-    <tableColumn name="Column15" id="15"/>
-    <tableColumn name="Column16" id="16"/>
-    <tableColumn name="Column17" id="17"/>
-    <tableColumn name="Column18" id="18"/>
-    <tableColumn name="Column19" id="19"/>
-    <tableColumn name="Column20" id="20"/>
-    <tableColumn name="Column21" id="21"/>
-    <tableColumn name="Column22" id="22"/>
-    <tableColumn name="Column23" id="23"/>
-    <tableColumn name="Column24" id="24"/>
-    <tableColumn name="Column25" id="25"/>
-    <tableColumn name="Column26" id="26"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Column8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Column9"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Column10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Column11"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Column12"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Column13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Column14"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Column15"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Column16"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Column17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Column18"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column24"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Column25"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Column26"/>
   </tableColumns>
-  <tableStyleInfo name="Hoja 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Hoja 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" headerRowCount="1"/>
@@ -168,7 +170,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -358,20 +360,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -390,31 +397,31 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>